<commit_message>
some old code move to other folder for now. all tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/milestone_data_output_test.xlsx
+++ b/tests/resources/milestone_data_output_test.xlsx
@@ -349,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,6 +388,11 @@
           <t>Baseline two</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">

</xml_diff>

<commit_message>
significant refactor of code in line with new group structure and MilestoneData class structure. All tests passing!
</commit_message>
<xml_diff>
--- a/tests/resources/milestone_data_output_test.xlsx
+++ b/tests/resources/milestone_data_output_test.xlsx
@@ -349,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,28 @@
       </c>
       <c r="F3" s="1" t="n"/>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Apollo 13</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Start of Construction/build</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>44586</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>44220</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>44220</v>
+      </c>
+      <c r="F4" s="1" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
milestones data, chart build and cli refactoring. Incomplete. resource added to dca analysis
</commit_message>
<xml_diff>
--- a/tests/resources/milestone_data_output_test.xlsx
+++ b/tests/resources/milestone_data_output_test.xlsx
@@ -349,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -397,7 +397,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Apollo 13</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -406,59 +406,536 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>36529</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>36528</v>
-      </c>
+        <v>36526</v>
+      </c>
+      <c r="D2" s="1" t="n"/>
       <c r="E2" s="1" t="n">
-        <v>36528</v>
+        <v>36526</v>
       </c>
       <c r="F2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Apollo 13</t>
+          <t>SoT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Standard A</t>
+          <t>Start of Project</t>
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>38504</v>
+        <v>36527</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>38504</v>
+        <v>36526</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>38504</v>
+        <v>36526</v>
       </c>
       <c r="F3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Apollo 13</t>
+          <t>A13</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Start of Project</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>36529</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>36528</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>36528</v>
+      </c>
+      <c r="F4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>F9</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Start of Project</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>36530</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>36529</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>36529</v>
+      </c>
+      <c r="F5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Columbia</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Start of Project</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>36531</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>36530</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>36530</v>
+      </c>
+      <c r="F6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>A13</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Standard A</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>38504</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>38504</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>38504</v>
+      </c>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Green lumber fallacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>A13</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Space Command</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>39081</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>39081</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>39081</v>
+      </c>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Memento mori and amor fati</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Columbia</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Standard A</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>41106</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>41106</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>41106</v>
+      </c>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>The mind is not a vessel to be filled but a fire to be lighted</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SoT</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Standard A</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>41153</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>41153</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>41153</v>
+      </c>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Green lumber fallacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SoT</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Inverted Cosmonauts</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>41537</v>
+      </c>
+      <c r="D11" s="1" t="n"/>
+      <c r="E11" s="1" t="n"/>
+      <c r="F11" s="1" t="n"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>The sea gets deeper the further you go into it</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>F9</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Standard A</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>41789</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>41789</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>41789</v>
+      </c>
+      <c r="F12" s="1" t="n"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>The sea gets deeper the further you go into it</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>F9</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Inverted Cosmonauts</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>41942</v>
+      </c>
+      <c r="D13" s="1" t="n"/>
+      <c r="E13" s="1" t="n"/>
+      <c r="F13" s="1" t="n"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>The sea gets deeper the further you go into it</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>F9</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Earth Command</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>42305</v>
+      </c>
+      <c r="D14" s="1" t="n"/>
+      <c r="E14" s="1" t="n"/>
+      <c r="F14" s="1" t="n"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Memento mori and amor fati</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Columbia</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Team Magma</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>42308</v>
+      </c>
+      <c r="D15" s="1" t="n"/>
+      <c r="E15" s="1" t="n"/>
+      <c r="F15" s="1" t="n"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Don't you know an apparition is just a cheap date. What have you been drinking these days</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mars</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Orbital Landing</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>43815</v>
+      </c>
+      <c r="D16" s="1" t="n"/>
+      <c r="E16" s="1" t="n">
+        <v>43815</v>
+      </c>
+      <c r="F16" s="1" t="n"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>The sea gets deeper the further you go into it</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mars</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Meteorite Shuttle</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>43900</v>
+      </c>
+      <c r="D17" s="1" t="n"/>
+      <c r="E17" s="1" t="n">
+        <v>43900</v>
+      </c>
+      <c r="F17" s="1" t="n"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>What you see if all there is</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Mars</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Tranquility Hypatia</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>44095</v>
+      </c>
+      <c r="D18" s="1" t="n"/>
+      <c r="E18" s="1" t="n">
+        <v>44095</v>
+      </c>
+      <c r="F18" s="1" t="n"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>What you see if all there is</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Mars</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>Start of Construction/build</t>
         </is>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C19" s="1" t="n">
+        <v>44583</v>
+      </c>
+      <c r="D19" s="1" t="n"/>
+      <c r="E19" s="1" t="n">
+        <v>44583</v>
+      </c>
+      <c r="F19" s="1" t="n"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>43th generation Roman</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SoT</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Start of Construction/build</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>44584</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>44218</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>44218</v>
+      </c>
+      <c r="F20" s="1" t="n"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Original </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>A13</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Start of Construction/build</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="n">
         <v>44586</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D21" s="1" t="n">
         <v>44220</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E21" s="1" t="n">
         <v>44220</v>
       </c>
-      <c r="F4" s="1" t="n"/>
+      <c r="F21" s="1" t="n"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Material </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>F9</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Start of Construction/build</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>44587</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>44221</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>44221</v>
+      </c>
+      <c r="F22" s="1" t="n"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">listening </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Columbia</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Start of Construction/build</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>44588</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>44222</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>44222</v>
+      </c>
+      <c r="F23" s="1" t="n"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>streets</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
wp refactor of tests. refactor json.py to json_file.py as was causing issues importing json library!
</commit_message>
<xml_diff>
--- a/tests/resources/milestone_data_output_test.xlsx
+++ b/tests/resources/milestone_data_output_test.xlsx
@@ -349,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -385,6 +385,16 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>bl_two</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>bl_three</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>Notes</t>
         </is>
       </c>
@@ -397,18 +407,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Start of Project</t>
+          <t>Sputnik Radiation</t>
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>36527</v>
+        <v>41537</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>36526</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>36526</v>
-      </c>
+        <v>41591</v>
+      </c>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -418,23 +428,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Standard A</t>
+          <t>Lunar Magma</t>
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>41153</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>41153</v>
-      </c>
+        <v>41537</v>
+      </c>
+      <c r="D3" s="1" t="n"/>
       <c r="E3" s="1" t="n">
-        <v>41153</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Don't you know an apparition is just a cheap date. What have you been drinking these days</t>
-        </is>
-      </c>
+        <v>41537</v>
+      </c>
+      <c r="F3" s="1" t="n"/>
+      <c r="G3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -444,14 +449,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Inverted Cosmonauts</t>
+          <t>Standard B</t>
         </is>
       </c>
       <c r="C4" s="1" t="n">
-        <v>41537</v>
-      </c>
-      <c r="D4" s="1" t="n"/>
-      <c r="E4" s="1" t="n"/>
+        <v>41571</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>41571</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>41571</v>
+      </c>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -461,23 +472,62 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Start of Construction/build</t>
+          <t>Standard C</t>
         </is>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44584</v>
+        <v>41571</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>44218</v>
+        <v>41571</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>44218</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>43th generation Roman</t>
-        </is>
-      </c>
+        <v>41537</v>
+      </c>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Sea of Tranquility</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Mercury Eleven</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>41591</v>
+      </c>
+      <c r="D6" s="1" t="n"/>
+      <c r="E6" s="1" t="n">
+        <v>41591</v>
+      </c>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sea of Tranquility</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Tranquility Radiation</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>41591</v>
+      </c>
+      <c r="D7" s="1" t="n"/>
+      <c r="E7" s="1" t="n">
+        <v>41537</v>
+      </c>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
full move to confi.ini file for data mgmt. tests updated. 2 failing. wp
</commit_message>
<xml_diff>
--- a/tests/resources/milestone_data_output_test.xlsx
+++ b/tests/resources/milestone_data_output_test.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,169 +433,289 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Report</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Milestone</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>current</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>last</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>bl_one</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>bl_two</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>bl_three</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Notes</t>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Status (top 250 ms)</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Escalated (top 250 cs)</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type (top 250 cs)</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Secured (top 250 cs)</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Notes / Central Response (top 250 cs)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sea of Tranquility</t>
+          <t>SoT</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>IPDC/GMPP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Milestone</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Sputnik Radiation</t>
         </is>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="E2" s="1" t="n">
         <v>41537</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="F2" s="1" t="n">
         <v>41591</v>
       </c>
-      <c r="E2" s="1" t="n"/>
-      <c r="F2" s="1" t="n"/>
       <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>What you see if all there is</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sea of Tranquility</t>
+          <t>SoT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>IPDC/GMPP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Milestone</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Lunar Magma</t>
         </is>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>41537</v>
-      </c>
-      <c r="D3" s="1" t="n"/>
       <c r="E3" s="1" t="n">
         <v>41537</v>
       </c>
       <c r="F3" s="1" t="n"/>
-      <c r="G3" s="1" t="n"/>
+      <c r="G3" s="1" t="n">
+        <v>41537</v>
+      </c>
+      <c r="H3" s="1" t="n"/>
+      <c r="I3" s="1" t="n"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>What you see if all there is</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sea of Tranquility</t>
+          <t>SoT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>IPDC/GMPP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Milestone</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Standard B</t>
         </is>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>41571</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>41571</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>41571</v>
       </c>
-      <c r="F4" s="1" t="n"/>
-      <c r="G4" s="1" t="n"/>
+      <c r="F4" s="1" t="n">
+        <v>41571</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>41571</v>
+      </c>
+      <c r="H4" s="1" t="n"/>
+      <c r="I4" s="1" t="n"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Memento mori and amor fati</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sea of Tranquility</t>
+          <t>SoT</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>IPDC/GMPP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Milestone</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>Standard C</t>
         </is>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="E5" s="1" t="n">
         <v>41571</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="F5" s="1" t="n">
         <v>41571</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="G5" s="1" t="n">
         <v>41537</v>
       </c>
-      <c r="F5" s="1" t="n"/>
-      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="1" t="n"/>
+      <c r="I5" s="1" t="n"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>What you see if all there is</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sea of Tranquility</t>
+          <t>SoT</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>IPDC/GMPP</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Milestone</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Mercury Eleven</t>
         </is>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>41591</v>
-      </c>
-      <c r="D6" s="1" t="n"/>
       <c r="E6" s="1" t="n">
         <v>41591</v>
       </c>
       <c r="F6" s="1" t="n"/>
-      <c r="G6" s="1" t="n"/>
+      <c r="G6" s="1" t="n">
+        <v>41591</v>
+      </c>
+      <c r="H6" s="1" t="n"/>
+      <c r="I6" s="1" t="n"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Memento mori and amor fati</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sea of Tranquility</t>
+          <t>SoT</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>IPDC/GMPP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Milestone</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Tranquility Radiation</t>
         </is>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="E7" s="1" t="n">
         <v>41591</v>
       </c>
-      <c r="D7" s="1" t="n"/>
-      <c r="E7" s="1" t="n">
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n">
         <v>41537</v>
       </c>
-      <c r="F7" s="1" t="n"/>
-      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
+      <c r="I7" s="1" t="n"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Memento mori and amor fati</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>